<commit_message>
Bismillah, tolong aku ya Allah.
</commit_message>
<xml_diff>
--- a/07. Direct Methode.xlsx
+++ b/07. Direct Methode.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Materi Kuliah\Semester 4\Metode Numerik\Metode Numerik Youtube\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Materi Kuliah\Semester 4\Metode Numerik\03. Metode Numerik Youtube\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FBEF4BD-793E-4B2A-9639-82DB70FE72A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E01A7D81-FE82-456D-9A8C-03E7ECC69EB5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{D5AD3D38-C285-47AD-9B62-FAA089E1E01A}"/>
   </bookViews>
@@ -30,6 +30,159 @@
     <t>AKAR-AKAR PERSAAMAAN KUADRAT DENGAN DIRECT METHODE</t>
   </si>
   <si>
+    <t>ɛ=0,0001</t>
+  </si>
+  <si>
+    <t>Iterasi</t>
+  </si>
+  <si>
+    <r>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ɛ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>a</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>%</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ɛ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>a</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>=|(x</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>i+1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-x</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>i</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)/x</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>i+1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>|</t>
+    </r>
+  </si>
+  <si>
     <r>
       <t>f(x)=x</t>
     </r>
@@ -40,248 +193,95 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
+      <t>³+x²</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-3x-3</t>
+    </r>
+  </si>
+  <si>
+    <t>x³+x²-3x-3=0</t>
+  </si>
+  <si>
+    <r>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>³=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-x</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>²+3x</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>+3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>x=(-x²+3x+3)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>⅓</t>
+    </r>
+  </si>
+  <si>
+    <t>Pengujian Nilai e</t>
+  </si>
+  <si>
+    <r>
+      <t>f(x)=-x</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
       <t>³+x²-3x-3</t>
     </r>
-  </si>
-  <si>
-    <t>ɛ=0,0001</t>
-  </si>
-  <si>
-    <t>Iterasi</t>
-  </si>
-  <si>
-    <r>
-      <t>x</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>x</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>2</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>ɛ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>a</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>%</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>ɛ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>a</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>=|(x</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>i+1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>-x</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>i</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>)/x</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>i+1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>|</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>f(x)=x</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>³+x²</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>-3x-3</t>
-    </r>
-  </si>
-  <si>
-    <t>x³+x²-3x-3=0</t>
-  </si>
-  <si>
-    <r>
-      <t>x</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>³=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>-x</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>²+3x</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>+3</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>x=(-x²+3x+3)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>⅓</t>
-    </r>
-  </si>
-  <si>
-    <t>Pengujian Nilai e</t>
   </si>
 </sst>
 </file>
@@ -695,7 +695,7 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -714,40 +714,40 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="I3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="I5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="E6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="4" t="s">
-        <v>6</v>
-      </c>
       <c r="F6" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
@@ -770,7 +770,7 @@
         <v>0</v>
       </c>
       <c r="I7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
@@ -795,7 +795,7 @@
         <v>0</v>
       </c>
       <c r="I8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">

</xml_diff>